<commit_message>
Pedagogical methods explained, new version
</commit_message>
<xml_diff>
--- a/sdd1_07/presentations/figures/organisation.xlsx
+++ b/sdd1_07/presentations/figures/organisation.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phgrosjean/Documents/Pgm/Github/BioDataScience-Course/sdd_lessons/sdd1_07/presentations/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906CF082-D9C6-3343-8801-8BDDA01958A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B765ED-E9E5-7449-B310-537F84BC949E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45300" yWindow="-5860" windowWidth="30240" windowHeight="18040" xr2:uid="{D3EBC074-A4FD-A749-B669-577D9CE817BF}"/>
+    <workbookView xWindow="33820" yWindow="-6220" windowWidth="37860" windowHeight="24940" activeTab="1" xr2:uid="{D3EBC074-A4FD-A749-B669-577D9CE817BF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Timing" sheetId="1" r:id="rId1"/>
+    <sheet name="Bloom" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Terminer
 les exercices</t>
@@ -70,13 +71,49 @@
   <si>
     <t>Faire des exercices avant
 d'assimiler la matière</t>
+  </si>
+  <si>
+    <t>2. Comprendre</t>
+  </si>
+  <si>
+    <t>3. Appliquer</t>
+  </si>
+  <si>
+    <t>4. Analyser</t>
+  </si>
+  <si>
+    <t>5. Évaluer</t>
+  </si>
+  <si>
+    <t>6. Créer</t>
+  </si>
+  <si>
+    <t>Processus cognitif</t>
+  </si>
+  <si>
+    <t>1. Mémoriser</t>
+  </si>
+  <si>
+    <t>Types de connaissances</t>
+  </si>
+  <si>
+    <t>A. factuelles</t>
+  </si>
+  <si>
+    <t>B. conceptuelles</t>
+  </si>
+  <si>
+    <t>C. procédurales</t>
+  </si>
+  <si>
+    <t>D. métacognitives</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -103,8 +140,16 @@
       <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,8 +198,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14996795556505021"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -162,53 +213,388 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -225,6 +611,292 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1247181</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>65052</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>228935</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>26952</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Oval 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFB6BBF0-B423-214F-A9E7-2568923EA310}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="1831994">
+          <a:off x="2074004" y="792656"/>
+          <a:ext cx="1812796" cy="1509713"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:br>
+            <a:rPr lang="en-GB" sz="1100"/>
+          </a:br>
+          <a:br>
+            <a:rPr lang="en-GB" sz="1100"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" baseline="0"/>
+            <a:t>      Bab1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>645290</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>248522</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1516430</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>429493</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Oval 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE5BED8D-44BD-884F-A3BD-AA30E20995F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="1971206">
+          <a:off x="2728884" y="1650814"/>
+          <a:ext cx="4019681" cy="2205033"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:br>
+            <a:rPr lang="en-GB" sz="1100"/>
+          </a:br>
+          <a:br>
+            <a:rPr lang="en-GB" sz="1100"/>
+          </a:br>
+          <a:br>
+            <a:rPr lang="en-GB" sz="1100"/>
+          </a:br>
+          <a:br>
+            <a:rPr lang="en-GB" sz="1100"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>         </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" baseline="0"/>
+            <a:t>Cours de Science des Données</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1434167</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>674191</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>22403</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>575662</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Oval 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11E6A127-B272-244D-81E9-1F7EAB73E1B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="1831994">
+          <a:off x="6666302" y="3425858"/>
+          <a:ext cx="1736778" cy="1250846"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:br>
+            <a:rPr lang="en-GB" sz="1100"/>
+          </a:br>
+          <a:br>
+            <a:rPr lang="en-GB" sz="1100"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>      </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" baseline="0"/>
+            <a:t>Doctorat</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>796721</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>402685</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1186927</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>130321</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Right Arrow 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E51300F-65AE-F549-A400-85F0A4D4F8E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="2104177">
+          <a:off x="4454586" y="1804977"/>
+          <a:ext cx="3538747" cy="402323"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent3">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -526,75 +1198,179 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D9B5ECB-EF7B-A946-9566-C49795BE57D4}">
   <dimension ref="B5:N8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="L8" sqref="L8:N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="5" spans="2:14" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="14" t="s">
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="11" t="s">
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="12"/>
-      <c r="J5" s="4" t="s">
+      <c r="I5" s="24"/>
+      <c r="J5" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="K5" s="3"/>
-      <c r="L5" s="6" t="s">
+      <c r="K5" s="26"/>
+      <c r="L5" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
     </row>
     <row r="8" spans="2:14" ht="58" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="10" t="s">
+      <c r="C8" s="30"/>
+      <c r="D8" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9" t="s">
+      <c r="E8" s="32"/>
+      <c r="F8" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="10" t="s">
+      <c r="G8" s="30"/>
+      <c r="H8" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="9" t="s">
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="L8:N8"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="L5:N5"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="L8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F341027-A206-7542-A59E-FBCFC32CBD4F}">
+  <dimension ref="B1:F9"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="192" zoomScaleNormal="192" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="3" max="6" width="20.6640625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="14"/>
+      <c r="C2" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="35"/>
+    </row>
+    <row r="3" spans="2:6" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="2:6" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="2:6" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="2:6" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="2:6" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="2:6" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>